<commit_message>
agregar a ID de Allan a excel
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t xml:space="preserve">nombre</t>
   </si>
@@ -62,6 +62,15 @@
   </si>
   <si>
     <t xml:space="preserve">ID41731117012891321440</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID89170112901440</t>
   </si>
 </sst>
 </file>
@@ -143,16 +152,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -169,120 +182,140 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="40.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="27.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="40.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="C2" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="C3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="C4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="C5" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregar apellidos, terminar comentarios y prueba de salida de imagen aleatoria
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,17 +20,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t xml:space="preserve">nombre</t>
   </si>
   <si>
+    <t xml:space="preserve">primer_apellido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">segundo_apellido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grado</t>
+  </si>
+  <si>
     <t xml:space="preserve">grupo</t>
   </si>
   <si>
-    <t xml:space="preserve">grado</t>
-  </si>
-  <si>
     <t xml:space="preserve">beca</t>
   </si>
   <si>
@@ -43,34 +49,31 @@
     <t xml:space="preserve">Johel</t>
   </si>
   <si>
+    <t xml:space="preserve">Hernadez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es asmatico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID41731117012891321440</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID89170112901440</t>
+  </si>
+  <si>
     <t xml:space="preserve">A</t>
   </si>
   <si>
-    <t xml:space="preserve">NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID41731117012891321441</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID41731117012891321442</t>
-  </si>
-  <si>
     <t xml:space="preserve">ID41731117012891321443</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Johel H R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID41731117012891321440</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID89170112901440</t>
   </si>
 </sst>
 </file>
@@ -152,7 +155,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -162,11 +165,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -182,30 +189,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="27.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="40.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="15.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="40.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -214,109 +222,111 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="F2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>10</v>
+      <c r="F3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>11</v>
+      <c r="G4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="H5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="H6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>